<commit_message>
switched left and right
</commit_message>
<xml_diff>
--- a/mic_positions/data/patch_plan.xlsx
+++ b/mic_positions/data/patch_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulbr\OneDrive\Documents\01 Uni OneDrive\13 WiSe 2425\02 MAP Microphone Array Project\Bassoon Project\02 Code\Bassoon2425\mic_positions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C87D4FD-CC5D-4F1D-AE07-307E2BAEE918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DE94BB-3B37-4D8E-B32B-167F86DDDC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="12390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F1A53D-CCA4-45AF-8DFC-9F7194F1B3CD}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -767,10 +767,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E2" s="12">
         <v>1</v>
@@ -784,10 +784,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E3" s="12">
         <v>2</v>
@@ -801,10 +801,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E4" s="12">
         <v>3</v>
@@ -818,10 +818,10 @@
         <v>10</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E5" s="12">
         <v>4</v>
@@ -835,10 +835,10 @@
         <v>11</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E6" s="12">
         <v>5</v>
@@ -852,10 +852,10 @@
         <v>12</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E7" s="12">
         <v>6</v>
@@ -869,10 +869,10 @@
         <v>13</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E8" s="12">
         <v>7</v>
@@ -886,10 +886,10 @@
         <v>14</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E9" s="12">
         <v>8</v>
@@ -903,10 +903,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E10" s="12">
         <v>9</v>
@@ -920,10 +920,10 @@
         <v>16</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E11" s="12">
         <v>10</v>
@@ -937,10 +937,10 @@
         <v>17</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E12" s="12">
         <v>11</v>
@@ -954,10 +954,10 @@
         <v>18</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E13" s="12">
         <v>12</v>
@@ -971,10 +971,10 @@
         <v>19</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E14" s="12">
         <v>13</v>
@@ -988,10 +988,10 @@
         <v>20</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E15" s="12">
         <v>14</v>
@@ -1005,10 +1005,10 @@
         <v>21</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E16" s="12">
         <v>15</v>
@@ -1022,10 +1022,10 @@
         <v>22</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E17" s="12">
         <v>16</v>
@@ -1039,7 +1039,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>77</v>
@@ -1345,10 +1345,10 @@
         <v>42</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E36" s="12">
         <v>1</v>
@@ -1362,10 +1362,10 @@
         <v>44</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E37" s="12">
         <v>2</v>
@@ -1379,10 +1379,10 @@
         <v>45</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E38" s="12">
         <v>3</v>
@@ -1396,10 +1396,10 @@
         <v>46</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E39" s="12">
         <v>4</v>
@@ -1413,10 +1413,10 @@
         <v>47</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E40" s="12">
         <v>5</v>
@@ -1430,10 +1430,10 @@
         <v>48</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E41" s="12">
         <v>6</v>
@@ -1447,10 +1447,10 @@
         <v>49</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E42" s="12">
         <v>7</v>
@@ -1464,10 +1464,10 @@
         <v>50</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E43" s="12">
         <v>8</v>
@@ -1481,10 +1481,10 @@
         <v>51</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E44" s="12">
         <v>9</v>
@@ -1498,10 +1498,10 @@
         <v>52</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E45" s="12">
         <v>10</v>
@@ -1515,10 +1515,10 @@
         <v>53</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E46" s="12">
         <v>11</v>
@@ -1532,10 +1532,10 @@
         <v>54</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E47" s="12">
         <v>12</v>
@@ -1549,10 +1549,10 @@
         <v>55</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E48" s="12">
         <v>13</v>
@@ -1566,10 +1566,10 @@
         <v>56</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E49" s="12">
         <v>14</v>
@@ -1583,10 +1583,10 @@
         <v>57</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E50" s="12">
         <v>15</v>
@@ -1600,10 +1600,10 @@
         <v>58</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E51" s="12">
         <v>16</v>
@@ -1617,7 +1617,7 @@
         <v>59</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D52" s="13" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
3d coords to xml
</commit_message>
<xml_diff>
--- a/mic_positions/data/patch_plan.xlsx
+++ b/mic_positions/data/patch_plan.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulbr\OneDrive\Documents\01 Uni OneDrive\13 WiSe 2425\02 MAP Microphone Array Project\Bassoon Project\02 Code\Bassoon2425\mic_positions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF51531E-468E-40E7-A381-CCADF5A0836E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B299C902-EA8C-4C8C-8B94-0AD423B30C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="12390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
+    <sheet name="old" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="74">
   <si>
     <t>Mic_Index</t>
   </si>
@@ -249,6 +250,12 @@
   </si>
   <si>
     <t>Channel</t>
+  </si>
+  <si>
+    <t>Stagebox_Channel</t>
+  </si>
+  <si>
+    <t>Array_Channel</t>
   </si>
 </sst>
 </file>
@@ -655,16 +662,1137 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F1A53D-CCA4-45AF-8DFC-9F7194F1B3CD}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="13.3984375" customWidth="1"/>
     <col min="2" max="5" width="11.19921875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E50" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E51" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E53" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E54" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E55" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E56" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E57" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E58" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E59" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E60" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E61" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E62" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E63" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E64" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E65" s="6">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28AC497-4867-4E51-91C8-4C00309BCD87}">
+  <dimension ref="A1:E65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>